<commit_message>
agregando emocion en frecuencia_promedio y comentando mlTutorial
</commit_message>
<xml_diff>
--- a/HallarVariables/00.xlsx
+++ b/HallarVariables/00.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Emocion</t>
   </si>
@@ -35,9 +35,6 @@
   </si>
   <si>
     <t>Subject</t>
-  </si>
-  <si>
-    <t>xx.xx</t>
   </si>
 </sst>
 </file>
@@ -399,11 +396,14 @@
       </c>
     </row>
     <row r="2" spans="1:7">
+      <c r="A2">
+        <v>0</v>
+      </c>
       <c r="B2">
         <v>880.1696386212914</v>
       </c>
-      <c r="C2" t="s">
-        <v>7</v>
+      <c r="C2">
+        <v>0</v>
       </c>
       <c r="D2">
         <v>2.0875625</v>

</xml_diff>